<commit_message>
Added settings menu to choose type file.
</commit_message>
<xml_diff>
--- a/REPORTS/report.xlsx
+++ b/REPORTS/report.xlsx
@@ -14,15 +14,15 @@
 </file>
 
 <file path=xl/SharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Акт сверка</t>
   </si>
   <si>
-    <t>за  01.09.2023 - 30.09.2023</t>
-  </si>
-  <si>
-    <t>MIS TRUBKA HARIDI UCHUN</t>
+    <t>за  01.10.2023 - 31.10.2023</t>
+  </si>
+  <si>
+    <t>Главный филиал контрагент</t>
   </si>
   <si>
     <t>№п/п</t>
@@ -46,22 +46,19 @@
     <t>Комментарий</t>
   </si>
   <si>
-    <t>Остаток</t>
-  </si>
-  <si>
     <t>Дт</t>
   </si>
   <si>
     <t>Кт</t>
   </si>
   <si>
-    <t>Остаток на 01.09.2023:</t>
+    <t>Остаток на 01.10.2023:</t>
   </si>
   <si>
     <t>Всего оборот:</t>
   </si>
   <si>
-    <t>Остаток на 30.09.2023:</t>
+    <t>Остаток на 31.10.2023:</t>
   </si>
 </sst>
 </file>
@@ -80,7 +77,7 @@
   <numFmts count="1">
     <numFmt numFmtId="50" formatCode=""/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <name val="Arial"/>
       <sz val="8"/>
@@ -120,9 +117,9 @@
       <charset val="0"/>
       <family val="2"/>
       <b val="true"/>
-      <i val="false"/>
-      <strike val="false"/>
-      <sz val="9"/>
+      <i val="true"/>
+      <strike val="false"/>
+      <sz val="10"/>
       <u val="none"/>
     </font>
     <font>
@@ -132,6 +129,7 @@
       <b val="true"/>
       <i val="true"/>
       <strike val="false"/>
+      <color rgb="0000FF"/>
       <sz val="10"/>
       <u val="none"/>
     </font>
@@ -142,29 +140,8 @@
       <b val="true"/>
       <i val="true"/>
       <strike val="false"/>
-      <color rgb="0000FF"/>
-      <sz val="10"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <family val="2"/>
-      <b val="true"/>
-      <i val="true"/>
-      <strike val="false"/>
       <color rgb="FF0000"/>
       <sz val="10"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <family val="2"/>
-      <b val="true"/>
-      <i val="true"/>
-      <strike val="false"/>
-      <sz val="8"/>
       <u val="none"/>
     </font>
   </fonts>
@@ -186,7 +163,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -235,71 +212,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="14">
     <xf/>
     <xf applyAlignment="true">
       <alignment horizontal="left"/>
@@ -319,46 +236,25 @@
     <xf fontId="3" fillId="2" borderId="3" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="4" fillId="2" borderId="4" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf fontId="4" fillId="2" borderId="3" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="4" fillId="2" borderId="5" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf fontId="5" fillId="2" borderId="3" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="3" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf fontId="7" fillId="2" borderId="3" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="right"/>
-    </xf>
     <xf fontId="6" fillId="2" borderId="3" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf fontId="8" fillId="2" borderId="6" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf fontId="8" fillId="2" borderId="7" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="4" fontId="6" fillId="2" borderId="3" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf fontId="4" fillId="3" borderId="3" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
     <xf fontId="5" fillId="3" borderId="3" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
     <xf fontId="6" fillId="3" borderId="3" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf fontId="7" fillId="3" borderId="3" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf fontId="8" fillId="3" borderId="6" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf fontId="8" fillId="3" borderId="7" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -380,7 +276,7 @@
     <outlinePr summaryBelow="false" summaryRight="false"/>
     <pageSetUpPr autoPageBreaks="false"/>
   </sheetPr>
-  <dimension ref="K8"/>
+  <dimension ref="I8"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0" rightToLeft="false"/>
   </sheetViews>
@@ -394,9 +290,7 @@
     <col min="6" max="6" width="17.16796875" style="1" customWidth="true"/>
     <col min="7" max="7" width="18.33203125" style="1" customWidth="true"/>
     <col min="8" max="8" width="20.83203125" style="1" customWidth="true"/>
-    <col min="9" max="9" width="37.33203125" style="1" customWidth="true"/>
-    <col min="10" max="10" width="13.66796875" style="1" customWidth="true"/>
-    <col min="11" max="11" width="10.5" style="1" customWidth="true"/>
+    <col min="9" max="9" width="25" style="1" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="true">
@@ -462,87 +356,71 @@
       <c r="I4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="7" t="e"/>
     </row>
     <row r="5" ht="13" customHeight="true">
       <c r="A5" s="4" t="e"/>
       <c r="B5" s="4" t="e"/>
       <c r="C5" s="4" t="e"/>
       <c r="D5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="F5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>12</v>
       </c>
       <c r="H5" s="4" t="e"/>
       <c r="I5" s="4" t="e"/>
-      <c r="J5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="6" ht="13" customHeight="true">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="7" t="e"/>
+      <c r="C6" s="7" t="e"/>
+      <c r="D6" s="8" t="e"/>
+      <c r="E6" s="9" t="e"/>
+      <c r="F6" s="8" t="e"/>
+      <c r="G6" s="10" t="n">
+        <v>757935.89</v>
+      </c>
+      <c r="H6" s="7" t="e"/>
+      <c r="I6" s="7" t="e"/>
+    </row>
+    <row r="7" ht="13" customHeight="true">
+      <c r="A7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="10" t="e"/>
-      <c r="C6" s="10" t="e"/>
-      <c r="D6" s="11" t="n">
-        <v>4</v>
-      </c>
-      <c r="E6" s="12" t="e"/>
-      <c r="F6" s="13" t="e"/>
-      <c r="G6" s="12" t="e"/>
-      <c r="H6" s="10" t="e"/>
-      <c r="I6" s="10" t="e"/>
-      <c r="J6" s="14" t="e"/>
-      <c r="K6" s="15" t="e"/>
-    </row>
-    <row r="7" ht="13" customHeight="true">
-      <c r="A7" s="16" t="s">
+      <c r="B7" s="11" t="e"/>
+      <c r="C7" s="11" t="e"/>
+      <c r="D7" s="12" t="e"/>
+      <c r="E7" s="13" t="e"/>
+      <c r="F7" s="12" t="e"/>
+      <c r="G7" s="13" t="e"/>
+      <c r="H7" s="11" t="e"/>
+      <c r="I7" s="11" t="e"/>
+    </row>
+    <row r="8" ht="13" customHeight="true">
+      <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="16" t="e"/>
-      <c r="C7" s="16" t="e"/>
-      <c r="D7" s="17" t="e"/>
-      <c r="E7" s="18" t="e"/>
-      <c r="F7" s="17" t="e"/>
-      <c r="G7" s="18" t="e"/>
-      <c r="H7" s="16" t="e"/>
-      <c r="I7" s="16" t="e"/>
-      <c r="J7" s="19" t="e"/>
-      <c r="K7" s="20" t="e"/>
-    </row>
-    <row r="8" ht="13" customHeight="true">
-      <c r="A8" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="10" t="e"/>
-      <c r="C8" s="10" t="e"/>
-      <c r="D8" s="11" t="n">
-        <v>4</v>
-      </c>
-      <c r="E8" s="12" t="e"/>
-      <c r="F8" s="13" t="e"/>
-      <c r="G8" s="12" t="e"/>
-      <c r="H8" s="10" t="e"/>
-      <c r="I8" s="10" t="e"/>
-      <c r="J8" s="14" t="e"/>
-      <c r="K8" s="15" t="e"/>
+      <c r="B8" s="7" t="e"/>
+      <c r="C8" s="7" t="e"/>
+      <c r="D8" s="8" t="e"/>
+      <c r="E8" s="9" t="e"/>
+      <c r="F8" s="8" t="e"/>
+      <c r="G8" s="10" t="n">
+        <v>757935.89</v>
+      </c>
+      <c r="H8" s="7" t="e"/>
+      <c r="I8" s="7" t="e"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="16">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:I3"/>
@@ -553,7 +431,6 @@
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="I4:I5"/>
-    <mergeCell ref="J4:K4"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="A7:C7"/>

</xml_diff>

<commit_message>
Added setting. In setting we can change language and type file format.
</commit_message>
<xml_diff>
--- a/REPORTS/report.xlsx
+++ b/REPORTS/report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/SharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Акт сверка</t>
   </si>
@@ -22,9 +22,6 @@
     <t>за  01.10.2023 - 31.10.2023</t>
   </si>
   <si>
-    <t>Главный филиал контрагент</t>
-  </si>
-  <si>
     <t>№п/п</t>
   </si>
   <si>
@@ -53,6 +50,30 @@
   </si>
   <si>
     <t>Остаток на 01.10.2023:</t>
+  </si>
+  <si>
+    <t>06.10.2023</t>
+  </si>
+  <si>
+    <t>Товар Кирим килиш №-1 553 858</t>
+  </si>
+  <si>
+    <t>Клиентларга пул бериш №-569 753</t>
+  </si>
+  <si>
+    <t>Поступление денег в банк №-3</t>
+  </si>
+  <si>
+    <t>Списание денег с банка №-2</t>
+  </si>
+  <si>
+    <t>Возврат продажа №-33</t>
+  </si>
+  <si>
+    <t>17.10.2023</t>
+  </si>
+  <si>
+    <t>Оптовая продажа №-111 830</t>
   </si>
   <si>
     <t>Всего оборот:</t>
@@ -74,10 +95,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="50" formatCode=""/>
+    <numFmt numFmtId="51" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <name val="Arial"/>
       <sz val="8"/>
@@ -141,6 +163,39 @@
       <i val="true"/>
       <strike val="false"/>
       <color rgb="FF0000"/>
+      <sz val="10"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <family val="2"/>
+      <b val="true"/>
+      <i val="false"/>
+      <strike val="false"/>
+      <color rgb="0000FF"/>
+      <sz val="10"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <family val="2"/>
+      <b val="true"/>
+      <i val="false"/>
+      <strike val="false"/>
+      <color rgb="FF0000"/>
+      <sz val="10"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <family val="2"/>
+      <b val="true"/>
+      <i val="false"/>
+      <strike val="false"/>
+      <color rgb="984E00"/>
       <sz val="10"/>
       <u val="none"/>
     </font>
@@ -216,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="30">
     <xf/>
     <xf applyAlignment="true">
       <alignment horizontal="left"/>
@@ -227,6 +282,9 @@
     <xf fontId="3" applyFont="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="3" applyNumberFormat="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
     <xf fontId="3" fillId="2" borderId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -245,16 +303,61 @@
     <xf fontId="6" fillId="2" borderId="3" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="1" fontId="3" borderId="3" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="3" borderId="3" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf fontId="3" borderId="3" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="7" borderId="3" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" borderId="3" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf fontId="8" borderId="3" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" borderId="3" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf fontId="9" borderId="3" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" borderId="3" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" borderId="3" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" borderId="3" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="51" fontId="7" borderId="3" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf fontId="4" fillId="3" borderId="3" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="3" borderId="3" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="3" borderId="3" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="3" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="3" borderId="3" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="2" borderId="3" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="4" fontId="6" fillId="2" borderId="3" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf fontId="4" fillId="3" borderId="3" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf fontId="5" fillId="3" borderId="3" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf fontId="6" fillId="3" borderId="3" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -276,7 +379,7 @@
     <outlinePr summaryBelow="false" summaryRight="false"/>
     <pageSetUpPr autoPageBreaks="false"/>
   </sheetPr>
-  <dimension ref="I8"/>
+  <dimension ref="I14"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0" rightToLeft="false"/>
   </sheetViews>
@@ -320,104 +423,240 @@
       <c r="I2" s="3" t="e"/>
     </row>
     <row r="3" ht="13" customHeight="true">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="n">
+        <v>711</v>
+      </c>
+      <c r="B3" s="4" t="e"/>
+      <c r="C3" s="4" t="e"/>
+      <c r="D3" s="4" t="e"/>
+      <c r="E3" s="4" t="e"/>
+      <c r="F3" s="4" t="e"/>
+      <c r="G3" s="4" t="e"/>
+      <c r="H3" s="4" t="e"/>
+      <c r="I3" s="4" t="e"/>
+    </row>
+    <row r="4" ht="13" customHeight="true">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="e"/>
-      <c r="C3" s="3" t="e"/>
-      <c r="D3" s="3" t="e"/>
-      <c r="E3" s="3" t="e"/>
-      <c r="F3" s="3" t="e"/>
-      <c r="G3" s="3" t="e"/>
-      <c r="H3" s="3" t="e"/>
-      <c r="I3" s="3" t="e"/>
-    </row>
-    <row r="4" ht="13" customHeight="true">
-      <c r="A4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="7" t="e"/>
+      <c r="F4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="6" t="e"/>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="7" t="e"/>
+      <c r="H4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="6" t="e"/>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="5" t="s">
+    </row>
+    <row r="5" ht="13" customHeight="true">
+      <c r="A5" s="5" t="e"/>
+      <c r="B5" s="5" t="e"/>
+      <c r="C5" s="5" t="e"/>
+      <c r="D5" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" ht="13" customHeight="true">
-      <c r="A5" s="4" t="e"/>
-      <c r="B5" s="4" t="e"/>
-      <c r="C5" s="4" t="e"/>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="5" t="e"/>
+      <c r="I5" s="5" t="e"/>
+    </row>
+    <row r="6" ht="13" customHeight="true">
+      <c r="A6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="4" t="e"/>
-      <c r="I5" s="4" t="e"/>
-    </row>
-    <row r="6" ht="13" customHeight="true">
-      <c r="A6" s="7" t="s">
+      <c r="B6" s="8" t="e"/>
+      <c r="C6" s="8" t="e"/>
+      <c r="D6" s="9" t="e"/>
+      <c r="E6" s="10" t="e"/>
+      <c r="F6" s="9" t="e"/>
+      <c r="G6" s="10" t="e"/>
+      <c r="H6" s="8" t="e"/>
+      <c r="I6" s="8" t="e"/>
+    </row>
+    <row r="7" ht="13" customHeight="true" s="1" customFormat="true">
+      <c r="A7" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="7" t="e"/>
-      <c r="C6" s="7" t="e"/>
-      <c r="D6" s="8" t="e"/>
-      <c r="E6" s="9" t="e"/>
-      <c r="F6" s="8" t="e"/>
-      <c r="G6" s="10" t="n">
-        <v>757935.89</v>
-      </c>
-      <c r="H6" s="7" t="e"/>
-      <c r="I6" s="7" t="e"/>
-    </row>
-    <row r="7" ht="13" customHeight="true">
-      <c r="A7" s="11" t="s">
+      <c r="C7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="11" t="e"/>
-      <c r="C7" s="11" t="e"/>
-      <c r="D7" s="12" t="e"/>
-      <c r="E7" s="13" t="e"/>
-      <c r="F7" s="12" t="e"/>
-      <c r="G7" s="13" t="e"/>
-      <c r="H7" s="11" t="e"/>
-      <c r="I7" s="11" t="e"/>
-    </row>
-    <row r="8" ht="13" customHeight="true">
-      <c r="A8" s="7" t="s">
+      <c r="D7" s="14" t="e"/>
+      <c r="E7" s="15" t="n">
+        <v>2292000</v>
+      </c>
+      <c r="F7" s="14" t="e"/>
+      <c r="G7" s="16" t="e"/>
+      <c r="H7" s="17" t="n">
+        <v>11460</v>
+      </c>
+      <c r="I7" s="18" t="e"/>
+    </row>
+    <row r="8" ht="13" customHeight="true" s="1" customFormat="true">
+      <c r="A8" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="7" t="e"/>
-      <c r="C8" s="7" t="e"/>
-      <c r="D8" s="8" t="e"/>
-      <c r="E8" s="9" t="e"/>
-      <c r="F8" s="8" t="e"/>
-      <c r="G8" s="10" t="n">
-        <v>757935.89</v>
-      </c>
-      <c r="H8" s="7" t="e"/>
-      <c r="I8" s="7" t="e"/>
+      <c r="D8" s="19" t="n">
+        <v>-2292000</v>
+      </c>
+      <c r="E8" s="16" t="e"/>
+      <c r="F8" s="20" t="n">
+        <v>202.18</v>
+      </c>
+      <c r="G8" s="16" t="e"/>
+      <c r="H8" s="17" t="n">
+        <v>11460</v>
+      </c>
+      <c r="I8" s="18" t="e"/>
+    </row>
+    <row r="9" ht="13" customHeight="true" s="1" customFormat="true">
+      <c r="A9" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="14" t="e"/>
+      <c r="E9" s="15" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="F9" s="14" t="e"/>
+      <c r="G9" s="16" t="e"/>
+      <c r="H9" s="17" t="n">
+        <v>11460</v>
+      </c>
+      <c r="I9" s="18" t="e"/>
+    </row>
+    <row r="10" ht="13" customHeight="true" s="1" customFormat="true">
+      <c r="A10" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="19" t="n">
+        <v>15000</v>
+      </c>
+      <c r="E10" s="16" t="e"/>
+      <c r="F10" s="14" t="e"/>
+      <c r="G10" s="16" t="e"/>
+      <c r="H10" s="17" t="n">
+        <v>11460</v>
+      </c>
+      <c r="I10" s="18" t="e"/>
+    </row>
+    <row r="11" ht="13" customHeight="true" s="1" customFormat="true">
+      <c r="A11" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="14" t="e"/>
+      <c r="E11" s="16" t="e"/>
+      <c r="F11" s="14" t="e"/>
+      <c r="G11" s="21" t="n">
+        <v>5510.82</v>
+      </c>
+      <c r="H11" s="17" t="n">
+        <v>11460</v>
+      </c>
+      <c r="I11" s="18" t="e"/>
+    </row>
+    <row r="12" ht="13" customHeight="true" s="1" customFormat="true">
+      <c r="A12" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="14" t="e"/>
+      <c r="E12" s="16" t="e"/>
+      <c r="F12" s="22" t="n">
+        <v>107.9</v>
+      </c>
+      <c r="G12" s="16" t="e"/>
+      <c r="H12" s="17" t="n">
+        <v>11460</v>
+      </c>
+      <c r="I12" s="18" t="e"/>
+    </row>
+    <row r="13" ht="13" customHeight="true">
+      <c r="A13" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="23" t="e"/>
+      <c r="C13" s="23" t="e"/>
+      <c r="D13" s="24" t="n">
+        <v>-2277000</v>
+      </c>
+      <c r="E13" s="25" t="n">
+        <v>3292000</v>
+      </c>
+      <c r="F13" s="26" t="n">
+        <v>310.08</v>
+      </c>
+      <c r="G13" s="27" t="n">
+        <v>5510.82</v>
+      </c>
+      <c r="H13" s="23" t="e"/>
+      <c r="I13" s="23" t="e"/>
+    </row>
+    <row r="14" ht="13" customHeight="true">
+      <c r="A14" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="8" t="e"/>
+      <c r="C14" s="8" t="e"/>
+      <c r="D14" s="9" t="e"/>
+      <c r="E14" s="28" t="n">
+        <v>5569000</v>
+      </c>
+      <c r="F14" s="9" t="e"/>
+      <c r="G14" s="29" t="n">
+        <v>5200.74</v>
+      </c>
+      <c r="H14" s="8" t="e"/>
+      <c r="I14" s="8" t="e"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -433,10 +672,10 @@
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="H6:I6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="H14:I14"/>
   </mergeCells>
   <pageMargins left="0.75" top="0.75" right="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>